<commit_message>
Route Dienstag erstellt + Funktionen
</commit_message>
<xml_diff>
--- a/Data/Montag/joined_Montag_coord_nn.xlsx
+++ b/Data/Montag/joined_Montag_coord_nn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Desktop\git_folder\DataScienceProject\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Desktop\git_folder\DataScienceProject\Data\Montag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807F394F-CD77-44A6-BD45-5A7297CFF06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BCB5A7-5AFA-433C-AA5B-C091A984DE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="176">
-  <si>
-    <t>NEUE_NAMEN_x</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="177">
   <si>
     <t>ADRESSE</t>
   </si>
@@ -548,6 +545,12 @@
   </si>
   <si>
     <t>KulturwikiOGD</t>
+  </si>
+  <si>
+    <t>NEUE_NAMEN</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,72 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -640,6 +708,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E71C7520-5D2E-4F65-9338-9F8DC38CAD39}" name="Table1" displayName="Table1" ref="A1:H56" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H56" xr:uid="{E71C7520-5D2E-4F65-9338-9F8DC38CAD39}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3D09986D-06E0-4401-9ABD-8654BFA93EA2}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{741CA6EC-CAE8-49E8-B84D-749F4F69D9E4}" name="NEUE_NAMEN"/>
+    <tableColumn id="3" xr3:uid="{52B9D9D1-159F-4A52-81D1-34DE20FEF7D5}" name="ADRESSE"/>
+    <tableColumn id="4" xr3:uid="{3B2A157A-DCD7-4A77-9B93-352DAA8019E5}" name="Sicherheit"/>
+    <tableColumn id="5" xr3:uid="{359574D4-9009-417E-96F2-26E65F4798EB}" name="Longitude_x"/>
+    <tableColumn id="6" xr3:uid="{7EA9FD9E-BE36-4470-8FDC-C165DFB85A89}" name="Latitude_x"/>
+    <tableColumn id="7" xr3:uid="{6525DA0D-2696-4882-B478-21110912BDC9}" name="Quelle"/>
+    <tableColumn id="8" xr3:uid="{15D66CF7-2C24-4934-923D-B8A0A6084D75}" name="URL"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -932,38 +1017,42 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
     <col min="3" max="5" width="29.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -971,13 +1060,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2">
         <v>16.4043687119417</v>
@@ -986,7 +1075,7 @@
         <v>48.185032303369297</v>
       </c>
       <c r="G2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -994,13 +1083,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E3">
         <v>16.4043687119417</v>
@@ -1009,7 +1098,7 @@
         <v>48.185032303369297</v>
       </c>
       <c r="G3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1017,22 +1106,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1040,22 +1129,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1063,22 +1152,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1086,22 +1175,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1109,13 +1198,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8">
         <v>16.370615999999998</v>
@@ -1124,10 +1213,10 @@
         <v>48.212879999999998</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1135,19 +1224,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1155,22 +1244,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1178,22 +1267,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1201,13 +1290,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E12">
         <v>16.371255519999998</v>
@@ -1216,7 +1305,7 @@
         <v>48.211645609999998</v>
       </c>
       <c r="G12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1224,13 +1313,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E13">
         <v>16.37105189</v>
@@ -1239,10 +1328,10 @@
         <v>48.212049499999999</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1250,13 +1339,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E14">
         <v>16.363849999999999</v>
@@ -1265,10 +1354,10 @@
         <v>48.208410000000001</v>
       </c>
       <c r="G14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1276,22 +1365,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1299,22 +1388,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1322,13 +1411,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" t="s">
         <v>170</v>
       </c>
-      <c r="C17" t="s">
-        <v>171</v>
-      </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1336,13 +1425,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E18">
         <v>16.368555000000001</v>
@@ -1351,10 +1440,10 @@
         <v>48.210929</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1362,22 +1451,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1385,22 +1474,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1408,22 +1497,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1431,13 +1520,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E22">
         <v>16.367861980000001</v>
@@ -1446,7 +1535,7 @@
         <v>48.21006182</v>
       </c>
       <c r="G22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1454,13 +1543,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23">
         <v>16.369923538928099</v>
@@ -1469,10 +1558,10 @@
         <v>48.210145667741003</v>
       </c>
       <c r="G23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H23" t="s">
         <v>148</v>
-      </c>
-      <c r="H23" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1480,22 +1569,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1503,22 +1592,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1526,22 +1615,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1549,7 +1638,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1557,22 +1646,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1580,22 +1669,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1603,13 +1692,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30">
         <v>16.371827634195402</v>
@@ -1618,7 +1707,7 @@
         <v>48.208506530717202</v>
       </c>
       <c r="G30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1626,22 +1715,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1649,22 +1738,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1672,22 +1761,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1695,22 +1784,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1718,10 +1807,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E35">
         <v>16.372171049999999</v>
@@ -1730,7 +1819,7 @@
         <v>48.211093990000002</v>
       </c>
       <c r="G35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1738,10 +1827,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1749,7 +1838,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1757,13 +1846,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E38">
         <v>16.375449110092202</v>
@@ -1772,7 +1861,7 @@
         <v>48.209044069322097</v>
       </c>
       <c r="G38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1780,10 +1869,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E39">
         <v>16.375679000000002</v>
@@ -1792,10 +1881,10 @@
         <v>48.208956000000001</v>
       </c>
       <c r="G39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -1803,22 +1892,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1826,13 +1915,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
         <v>163</v>
-      </c>
-      <c r="D41" t="s">
-        <v>164</v>
       </c>
       <c r="E41">
         <v>16.378137599764798</v>
@@ -1841,10 +1930,10 @@
         <v>48.208884619743301</v>
       </c>
       <c r="G41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1852,13 +1941,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E42">
         <v>16.377677354271398</v>
@@ -1867,10 +1956,10 @@
         <v>48.208837970142497</v>
       </c>
       <c r="G42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1878,13 +1967,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1892,7 +1981,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -1900,13 +1989,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E45">
         <v>16.37723433</v>
@@ -1915,7 +2004,7 @@
         <v>48.209185769999998</v>
       </c>
       <c r="G45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1923,13 +2012,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E46">
         <v>16.370856849999999</v>
@@ -1938,7 +2027,7 @@
         <v>48.211275399999998</v>
       </c>
       <c r="G46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -1946,7 +2035,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -1954,22 +2043,22 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -1977,7 +2066,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -1985,13 +2074,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E50">
         <v>16.3774172646315</v>
@@ -2000,10 +2089,10 @@
         <v>48.210834889438999</v>
       </c>
       <c r="G50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2011,10 +2100,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E51">
         <v>16.379059999999999</v>
@@ -2023,7 +2112,7 @@
         <v>48.210194999999999</v>
       </c>
       <c r="G51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2031,13 +2120,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52">
         <v>16.378716273853101</v>
@@ -2046,10 +2135,10 @@
         <v>48.2100720501452</v>
       </c>
       <c r="G52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -2057,13 +2146,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E53">
         <v>16.358228749999999</v>
@@ -2072,7 +2161,7 @@
         <v>48.218601169999999</v>
       </c>
       <c r="G53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -2080,13 +2169,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E54">
         <v>16.363210696599701</v>
@@ -2095,7 +2184,7 @@
         <v>48.2095940666158</v>
       </c>
       <c r="G54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -2103,22 +2192,22 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2126,25 +2215,28 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>